<commit_message>
master: just need to figure out FoodCode, fixed recipes within recipes
</commit_message>
<xml_diff>
--- a/data/1-Premade food nutrition.xlsx
+++ b/data/1-Premade food nutrition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryans\PycharmProjects\menu-cnf-lookup\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\PycharmProjects\menu-cnf-lookup\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF9F79-05DF-4200-8430-B22E6AD65B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C754A786-37B7-4DE0-AD5D-5BE02224EF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{8E9FFF68-D619-42D1-AEC0-B80AB13FA822}"/>
+    <workbookView xWindow="40515" yWindow="6915" windowWidth="28800" windowHeight="15435" xr2:uid="{8E9FFF68-D619-42D1-AEC0-B80AB13FA822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Iron (mg)</t>
   </si>
   <si>
-    <t xml:space="preserve">chickpeas </t>
-  </si>
-  <si>
     <t>ml</t>
   </si>
   <si>
@@ -111,49 +108,52 @@
     <t xml:space="preserve">g </t>
   </si>
   <si>
-    <t xml:space="preserve">shredded cheese </t>
-  </si>
-  <si>
-    <t>Whole Wheat Wrap</t>
-  </si>
-  <si>
     <t>olive oil</t>
   </si>
   <si>
-    <t>Smoked Mozarella</t>
-  </si>
-  <si>
-    <t>Goat Cheese</t>
-  </si>
-  <si>
-    <t>Brie Cheese</t>
-  </si>
-  <si>
     <t>Tofu</t>
   </si>
   <si>
-    <t xml:space="preserve">Multigrain Ciabatta </t>
-  </si>
-  <si>
     <t>canola oil</t>
   </si>
   <si>
-    <t>Smoked Salmon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honey mustard </t>
-  </si>
-  <si>
     <t>caper berries</t>
   </si>
   <si>
-    <t xml:space="preserve">sumac </t>
-  </si>
-  <si>
-    <t>Prosciutto</t>
-  </si>
-  <si>
     <t>Tuna</t>
+  </si>
+  <si>
+    <t>sumac</t>
+  </si>
+  <si>
+    <t>Honey mustard</t>
+  </si>
+  <si>
+    <t>chickpeas</t>
+  </si>
+  <si>
+    <t>shredded cheese</t>
+  </si>
+  <si>
+    <t>goat cheese</t>
+  </si>
+  <si>
+    <t>brie cheese</t>
+  </si>
+  <si>
+    <t>whole wheat wrap</t>
+  </si>
+  <si>
+    <t>smoked mozzarella</t>
+  </si>
+  <si>
+    <t>multigrain ciabatta</t>
+  </si>
+  <si>
+    <t>prosciutto</t>
+  </si>
+  <si>
+    <t>smoked salmon</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,10 +568,10 @@
         <v>13</v>
       </c>
       <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
         <v>20</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>104</v>
@@ -635,13 +635,13 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -688,13 +688,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>35</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>16</v>
@@ -794,13 +794,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>819</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>30.4</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>85</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>30</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>30</v>
@@ -1165,13 +1165,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>100</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16">
         <v>110</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -1377,13 +1377,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>80</v>
@@ -1430,13 +1430,13 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>100</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>110</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>100</v>

</xml_diff>